<commit_message>
Double Dragon - spreadsheet filled out and some very insignificant tasing
</commit_message>
<xml_diff>
--- a/DoubleDragon/DD.xlsx
+++ b/DoubleDragon/DD.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="220">
   <si>
     <t>Notes</t>
   </si>
@@ -708,6 +708,18 @@
   <si>
     <t>Phil</t>
   </si>
+  <si>
+    <t>Cutscene appears</t>
+  </si>
+  <si>
+    <t>Bimmy Appears</t>
+  </si>
+  <si>
+    <t>Enemy Set 2 - Screen Scroll</t>
+  </si>
+  <si>
+    <t>Enemy Set 1 - Screen Scroll</t>
+  </si>
 </sst>
 </file>
 
@@ -717,10 +729,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
@@ -1625,34 +1644,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1660,208 +1679,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1871,10 +1890,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1895,133 +1914,136 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2340,8 +2362,8 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2483,7 +2505,7 @@
       <c r="E7" s="93"/>
       <c r="F7" s="93"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="156" t="s">
         <v>188</v>
       </c>
@@ -2503,28 +2525,38 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="149"/>
       <c r="B9" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
+      <c r="C9" s="99">
+        <v>0</v>
+      </c>
+      <c r="D9" s="99">
+        <v>0</v>
+      </c>
       <c r="E9" s="99"/>
       <c r="F9" s="104"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="149"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
+      <c r="B10" s="212" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="101">
+        <v>21</v>
+      </c>
+      <c r="D10" s="101">
+        <v>21</v>
+      </c>
       <c r="E10" s="101">
         <f t="shared" ref="E10:E16" si="0">IF(AND(C10&gt;0,D10&gt;0), D10-C10, 0)</f>
         <v>0</v>
       </c>
       <c r="F10" s="105"/>
     </row>
-    <row r="11" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="149"/>
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
@@ -2535,7 +2567,7 @@
       </c>
       <c r="F11" s="105"/>
     </row>
-    <row r="12" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="149"/>
       <c r="B12" s="100"/>
       <c r="C12" s="101"/>
@@ -2546,7 +2578,7 @@
       </c>
       <c r="F12" s="105"/>
     </row>
-    <row r="13" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="149"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
@@ -2557,7 +2589,7 @@
       </c>
       <c r="F13" s="105"/>
     </row>
-    <row r="14" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="149"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
@@ -2568,27 +2600,33 @@
       </c>
       <c r="F14" s="105"/>
     </row>
-    <row r="15" spans="1:11" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="149"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
+      <c r="B15" s="212" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="101">
+        <v>949</v>
+      </c>
+      <c r="D15" s="101">
+        <v>949</v>
+      </c>
       <c r="E15" s="121">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15" s="105"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="149"/>
       <c r="B16" s="98" t="s">
         <v>187</v>
       </c>
       <c r="C16" s="99">
-        <v>0</v>
+        <v>949</v>
       </c>
       <c r="D16" s="99">
-        <v>0</v>
+        <v>949</v>
       </c>
       <c r="E16" s="101">
         <f t="shared" si="0"/>
@@ -2596,7 +2634,7 @@
       </c>
       <c r="F16" s="104"/>
     </row>
-    <row r="17" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="116" t="s">
         <v>190</v>
       </c>
@@ -2605,11 +2643,11 @@
       </c>
       <c r="C17" s="103">
         <f>C16-C9</f>
-        <v>0</v>
+        <v>949</v>
       </c>
       <c r="D17" s="103">
         <f>D16-D9</f>
-        <v>0</v>
+        <v>949</v>
       </c>
       <c r="E17" s="122">
         <f>E16-E9</f>
@@ -2622,7 +2660,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="150" t="s">
         <v>168</v>
       </c>
@@ -2642,53 +2680,75 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="149"/>
       <c r="B20" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
+      <c r="C20" s="99">
+        <v>949</v>
+      </c>
+      <c r="D20" s="99">
+        <v>949</v>
+      </c>
       <c r="E20" s="123">
         <f t="shared" ref="E20:E33" si="1">IF(AND(C20&gt;0,D20&gt;0), D20-C20, 0)</f>
         <v>0</v>
       </c>
       <c r="F20" s="104"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="149"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="101"/>
+      <c r="B21" s="212" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" s="101">
+        <v>949</v>
+      </c>
+      <c r="D21" s="101">
+        <v>949</v>
+      </c>
       <c r="E21" s="124">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F21" s="105"/>
     </row>
-    <row r="22" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="149"/>
-      <c r="B22" s="100"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
+      <c r="B22" s="212" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22" s="101">
+        <v>1553</v>
+      </c>
+      <c r="D22" s="101">
+        <v>1559</v>
+      </c>
       <c r="E22" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F22" s="105"/>
     </row>
-    <row r="23" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="149"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
+      <c r="B23" s="212" t="s">
+        <v>218</v>
+      </c>
+      <c r="C23" s="101">
+        <v>2121</v>
+      </c>
+      <c r="D23" s="101">
+        <v>2125</v>
+      </c>
       <c r="E23" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F23" s="105"/>
     </row>
-    <row r="24" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="149"/>
       <c r="B24" s="100"/>
       <c r="C24" s="101"/>
@@ -2699,7 +2759,7 @@
       </c>
       <c r="F24" s="105"/>
     </row>
-    <row r="25" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="149"/>
       <c r="B25" s="100"/>
       <c r="C25" s="101"/>
@@ -2710,7 +2770,7 @@
       </c>
       <c r="F25" s="105"/>
     </row>
-    <row r="26" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="149"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
@@ -2721,7 +2781,7 @@
       </c>
       <c r="F26" s="105"/>
     </row>
-    <row r="27" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="149"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
@@ -2732,7 +2792,7 @@
       </c>
       <c r="F27" s="105"/>
     </row>
-    <row r="28" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="149"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
@@ -2743,7 +2803,7 @@
       </c>
       <c r="F28" s="105"/>
     </row>
-    <row r="29" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="149"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
@@ -2754,7 +2814,7 @@
       </c>
       <c r="F29" s="105"/>
     </row>
-    <row r="30" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="149"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
@@ -2765,7 +2825,7 @@
       </c>
       <c r="F30" s="105"/>
     </row>
-    <row r="31" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="149"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
@@ -2776,7 +2836,7 @@
       </c>
       <c r="F31" s="105"/>
     </row>
-    <row r="32" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="149"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
@@ -2787,7 +2847,7 @@
       </c>
       <c r="F32" s="105"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="149"/>
       <c r="B33" s="98" t="s">
         <v>187</v>
@@ -2800,7 +2860,7 @@
       </c>
       <c r="F33" s="104"/>
     </row>
-    <row r="34" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="117">
         <v>1</v>
       </c>
@@ -2809,11 +2869,11 @@
       </c>
       <c r="C34" s="103">
         <f>C33-C20</f>
-        <v>0</v>
+        <v>-949</v>
       </c>
       <c r="D34" s="103">
         <f>D33-D20</f>
-        <v>0</v>
+        <v>-949</v>
       </c>
       <c r="E34" s="126">
         <f>E33-E20</f>
@@ -4155,11 +4215,6 @@
     <row r="150" spans="1:6" collapsed="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A103:A117"/>
-    <mergeCell ref="A70:A84"/>
-    <mergeCell ref="A119:A133"/>
-    <mergeCell ref="A87:A101"/>
     <mergeCell ref="A36:A50"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="C5:D5"/>
@@ -4168,6 +4223,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A103:A117"/>
+    <mergeCell ref="A70:A84"/>
+    <mergeCell ref="A119:A133"/>
+    <mergeCell ref="A87:A101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4199,13 +4259,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="175" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4235,18 +4295,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="159"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4398,9 +4458,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="162"/>
-      <c r="D21" s="163"/>
-      <c r="E21" s="163"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="160"/>
+      <c r="E21" s="160"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4551,9 +4611,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="160"/>
-      <c r="D38" s="161"/>
-      <c r="E38" s="161"/>
+      <c r="C38" s="157"/>
+      <c r="D38" s="158"/>
+      <c r="E38" s="158"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -4704,9 +4764,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="160"/>
-      <c r="D55" s="161"/>
-      <c r="E55" s="161"/>
+      <c r="C55" s="157"/>
+      <c r="D55" s="158"/>
+      <c r="E55" s="158"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -4857,9 +4917,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="160"/>
-      <c r="D72" s="161"/>
-      <c r="E72" s="161"/>
+      <c r="C72" s="157"/>
+      <c r="D72" s="158"/>
+      <c r="E72" s="158"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5010,9 +5070,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="160"/>
-      <c r="D89" s="161"/>
-      <c r="E89" s="161"/>
+      <c r="C89" s="157"/>
+      <c r="D89" s="158"/>
+      <c r="E89" s="158"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5163,9 +5223,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="160"/>
-      <c r="D106" s="161"/>
-      <c r="E106" s="161"/>
+      <c r="C106" s="157"/>
+      <c r="D106" s="158"/>
+      <c r="E106" s="158"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5316,9 +5376,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="160"/>
-      <c r="D123" s="161"/>
-      <c r="E123" s="161"/>
+      <c r="C123" s="157"/>
+      <c r="D123" s="158"/>
+      <c r="E123" s="158"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5469,9 +5529,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="160"/>
-      <c r="D140" s="161"/>
-      <c r="E140" s="161"/>
+      <c r="C140" s="157"/>
+      <c r="D140" s="158"/>
+      <c r="E140" s="158"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -5622,9 +5682,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="160"/>
-      <c r="D157" s="161"/>
-      <c r="E157" s="161"/>
+      <c r="C157" s="157"/>
+      <c r="D157" s="158"/>
+      <c r="E157" s="158"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -5775,9 +5835,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="160"/>
-      <c r="D174" s="161"/>
-      <c r="E174" s="161"/>
+      <c r="C174" s="157"/>
+      <c r="D174" s="158"/>
+      <c r="E174" s="158"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -5928,9 +5988,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="160"/>
-      <c r="D191" s="161"/>
-      <c r="E191" s="161"/>
+      <c r="C191" s="157"/>
+      <c r="D191" s="158"/>
+      <c r="E191" s="158"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6081,9 +6141,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="160"/>
-      <c r="D208" s="161"/>
-      <c r="E208" s="161"/>
+      <c r="C208" s="157"/>
+      <c r="D208" s="158"/>
+      <c r="E208" s="158"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6234,9 +6294,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="160"/>
-      <c r="D225" s="161"/>
-      <c r="E225" s="161"/>
+      <c r="C225" s="157"/>
+      <c r="D225" s="158"/>
+      <c r="E225" s="158"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6387,9 +6447,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="160"/>
-      <c r="D242" s="161"/>
-      <c r="E242" s="161"/>
+      <c r="C242" s="157"/>
+      <c r="D242" s="158"/>
+      <c r="E242" s="158"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6540,9 +6600,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="160"/>
-      <c r="D259" s="161"/>
-      <c r="E259" s="161"/>
+      <c r="C259" s="157"/>
+      <c r="D259" s="158"/>
+      <c r="E259" s="158"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -6693,18 +6753,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="164"/>
-      <c r="D276" s="165"/>
-      <c r="E276" s="165"/>
+      <c r="C276" s="173"/>
+      <c r="D276" s="174"/>
+      <c r="E276" s="174"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="160"/>
-      <c r="D277" s="161"/>
-      <c r="E277" s="161"/>
+      <c r="C277" s="157"/>
+      <c r="D277" s="158"/>
+      <c r="E277" s="158"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -6855,9 +6915,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="162"/>
-      <c r="D294" s="163"/>
-      <c r="E294" s="163"/>
+      <c r="C294" s="159"/>
+      <c r="D294" s="160"/>
+      <c r="E294" s="160"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7008,9 +7068,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="160"/>
-      <c r="D311" s="161"/>
-      <c r="E311" s="161"/>
+      <c r="C311" s="157"/>
+      <c r="D311" s="158"/>
+      <c r="E311" s="158"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7161,9 +7221,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="160"/>
-      <c r="D328" s="161"/>
-      <c r="E328" s="161"/>
+      <c r="C328" s="157"/>
+      <c r="D328" s="158"/>
+      <c r="E328" s="158"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7314,9 +7374,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="160"/>
-      <c r="D345" s="161"/>
-      <c r="E345" s="161"/>
+      <c r="C345" s="157"/>
+      <c r="D345" s="158"/>
+      <c r="E345" s="158"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7467,9 +7527,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="160"/>
-      <c r="D362" s="161"/>
-      <c r="E362" s="161"/>
+      <c r="C362" s="157"/>
+      <c r="D362" s="158"/>
+      <c r="E362" s="158"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7620,9 +7680,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="160"/>
-      <c r="D379" s="161"/>
-      <c r="E379" s="161"/>
+      <c r="C379" s="157"/>
+      <c r="D379" s="158"/>
+      <c r="E379" s="158"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -7773,9 +7833,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="160"/>
-      <c r="D396" s="161"/>
-      <c r="E396" s="161"/>
+      <c r="C396" s="157"/>
+      <c r="D396" s="158"/>
+      <c r="E396" s="158"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -7926,9 +7986,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="160"/>
-      <c r="D413" s="161"/>
-      <c r="E413" s="161"/>
+      <c r="C413" s="157"/>
+      <c r="D413" s="158"/>
+      <c r="E413" s="158"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8079,9 +8139,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="160"/>
-      <c r="D430" s="161"/>
-      <c r="E430" s="161"/>
+      <c r="C430" s="157"/>
+      <c r="D430" s="158"/>
+      <c r="E430" s="158"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8232,9 +8292,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="160"/>
-      <c r="D447" s="161"/>
-      <c r="E447" s="161"/>
+      <c r="C447" s="157"/>
+      <c r="D447" s="158"/>
+      <c r="E447" s="158"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8385,9 +8445,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="160"/>
-      <c r="D464" s="161"/>
-      <c r="E464" s="161"/>
+      <c r="C464" s="157"/>
+      <c r="D464" s="158"/>
+      <c r="E464" s="158"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8538,9 +8598,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="160"/>
-      <c r="D481" s="161"/>
-      <c r="E481" s="161"/>
+      <c r="C481" s="157"/>
+      <c r="D481" s="158"/>
+      <c r="E481" s="158"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -8691,9 +8751,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="160"/>
-      <c r="D498" s="161"/>
-      <c r="E498" s="161"/>
+      <c r="C498" s="157"/>
+      <c r="D498" s="158"/>
+      <c r="E498" s="158"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -8844,9 +8904,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="160"/>
-      <c r="D515" s="161"/>
-      <c r="E515" s="161"/>
+      <c r="C515" s="157"/>
+      <c r="D515" s="158"/>
+      <c r="E515" s="158"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -8997,9 +9057,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="160"/>
-      <c r="D532" s="161"/>
-      <c r="E532" s="161"/>
+      <c r="C532" s="157"/>
+      <c r="D532" s="158"/>
+      <c r="E532" s="158"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9150,18 +9210,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="166"/>
-      <c r="D549" s="167"/>
-      <c r="E549" s="167"/>
+      <c r="C549" s="171"/>
+      <c r="D549" s="172"/>
+      <c r="E549" s="172"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="160"/>
-      <c r="D550" s="161"/>
-      <c r="E550" s="161"/>
+      <c r="C550" s="157"/>
+      <c r="D550" s="158"/>
+      <c r="E550" s="158"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9312,9 +9372,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="162"/>
-      <c r="D567" s="163"/>
-      <c r="E567" s="163"/>
+      <c r="C567" s="159"/>
+      <c r="D567" s="160"/>
+      <c r="E567" s="160"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9465,9 +9525,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="160"/>
-      <c r="D584" s="161"/>
-      <c r="E584" s="161"/>
+      <c r="C584" s="157"/>
+      <c r="D584" s="158"/>
+      <c r="E584" s="158"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9618,9 +9678,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="160"/>
-      <c r="D601" s="161"/>
-      <c r="E601" s="161"/>
+      <c r="C601" s="157"/>
+      <c r="D601" s="158"/>
+      <c r="E601" s="158"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -9771,9 +9831,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="160"/>
-      <c r="D618" s="161"/>
-      <c r="E618" s="161"/>
+      <c r="C618" s="157"/>
+      <c r="D618" s="158"/>
+      <c r="E618" s="158"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -9924,9 +9984,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="160"/>
-      <c r="D635" s="161"/>
-      <c r="E635" s="161"/>
+      <c r="C635" s="157"/>
+      <c r="D635" s="158"/>
+      <c r="E635" s="158"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10077,9 +10137,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="160"/>
-      <c r="D652" s="161"/>
-      <c r="E652" s="161"/>
+      <c r="C652" s="157"/>
+      <c r="D652" s="158"/>
+      <c r="E652" s="158"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10230,9 +10290,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="160"/>
-      <c r="D669" s="161"/>
-      <c r="E669" s="161"/>
+      <c r="C669" s="157"/>
+      <c r="D669" s="158"/>
+      <c r="E669" s="158"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10383,9 +10443,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="160"/>
-      <c r="D686" s="161"/>
-      <c r="E686" s="161"/>
+      <c r="C686" s="157"/>
+      <c r="D686" s="158"/>
+      <c r="E686" s="158"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10536,9 +10596,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="160"/>
-      <c r="D703" s="161"/>
-      <c r="E703" s="161"/>
+      <c r="C703" s="157"/>
+      <c r="D703" s="158"/>
+      <c r="E703" s="158"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -10689,9 +10749,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="160"/>
-      <c r="D720" s="161"/>
-      <c r="E720" s="161"/>
+      <c r="C720" s="157"/>
+      <c r="D720" s="158"/>
+      <c r="E720" s="158"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -10842,9 +10902,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="160"/>
-      <c r="D737" s="161"/>
-      <c r="E737" s="161"/>
+      <c r="C737" s="157"/>
+      <c r="D737" s="158"/>
+      <c r="E737" s="158"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -10995,9 +11055,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="160"/>
-      <c r="D754" s="161"/>
-      <c r="E754" s="161"/>
+      <c r="C754" s="157"/>
+      <c r="D754" s="158"/>
+      <c r="E754" s="158"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11148,9 +11208,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="160"/>
-      <c r="D771" s="161"/>
-      <c r="E771" s="161"/>
+      <c r="C771" s="157"/>
+      <c r="D771" s="158"/>
+      <c r="E771" s="158"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11301,9 +11361,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="160"/>
-      <c r="D788" s="161"/>
-      <c r="E788" s="161"/>
+      <c r="C788" s="157"/>
+      <c r="D788" s="158"/>
+      <c r="E788" s="158"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11454,9 +11514,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="160"/>
-      <c r="D805" s="161"/>
-      <c r="E805" s="161"/>
+      <c r="C805" s="157"/>
+      <c r="D805" s="158"/>
+      <c r="E805" s="158"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11607,18 +11667,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="168"/>
-      <c r="D822" s="169"/>
-      <c r="E822" s="169"/>
+      <c r="C822" s="169"/>
+      <c r="D822" s="170"/>
+      <c r="E822" s="170"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="160"/>
-      <c r="D823" s="161"/>
-      <c r="E823" s="161"/>
+      <c r="C823" s="157"/>
+      <c r="D823" s="158"/>
+      <c r="E823" s="158"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -11769,9 +11829,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="162"/>
-      <c r="D840" s="163"/>
-      <c r="E840" s="163"/>
+      <c r="C840" s="159"/>
+      <c r="D840" s="160"/>
+      <c r="E840" s="160"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -11922,9 +11982,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="160"/>
-      <c r="D857" s="161"/>
-      <c r="E857" s="161"/>
+      <c r="C857" s="157"/>
+      <c r="D857" s="158"/>
+      <c r="E857" s="158"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12075,9 +12135,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="160"/>
-      <c r="D874" s="161"/>
-      <c r="E874" s="161"/>
+      <c r="C874" s="157"/>
+      <c r="D874" s="158"/>
+      <c r="E874" s="158"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12228,9 +12288,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="160"/>
-      <c r="D891" s="161"/>
-      <c r="E891" s="161"/>
+      <c r="C891" s="157"/>
+      <c r="D891" s="158"/>
+      <c r="E891" s="158"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12381,9 +12441,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="160"/>
-      <c r="D908" s="161"/>
-      <c r="E908" s="161"/>
+      <c r="C908" s="157"/>
+      <c r="D908" s="158"/>
+      <c r="E908" s="158"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12534,9 +12594,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="160"/>
-      <c r="D925" s="161"/>
-      <c r="E925" s="161"/>
+      <c r="C925" s="157"/>
+      <c r="D925" s="158"/>
+      <c r="E925" s="158"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -12687,9 +12747,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="160"/>
-      <c r="D942" s="161"/>
-      <c r="E942" s="161"/>
+      <c r="C942" s="157"/>
+      <c r="D942" s="158"/>
+      <c r="E942" s="158"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -12840,9 +12900,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="160"/>
-      <c r="D959" s="161"/>
-      <c r="E959" s="161"/>
+      <c r="C959" s="157"/>
+      <c r="D959" s="158"/>
+      <c r="E959" s="158"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -12993,9 +13053,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="160"/>
-      <c r="D976" s="161"/>
-      <c r="E976" s="161"/>
+      <c r="C976" s="157"/>
+      <c r="D976" s="158"/>
+      <c r="E976" s="158"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13146,9 +13206,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="160"/>
-      <c r="D993" s="161"/>
-      <c r="E993" s="161"/>
+      <c r="C993" s="157"/>
+      <c r="D993" s="158"/>
+      <c r="E993" s="158"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13299,9 +13359,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="160"/>
-      <c r="D1010" s="161"/>
-      <c r="E1010" s="161"/>
+      <c r="C1010" s="157"/>
+      <c r="D1010" s="158"/>
+      <c r="E1010" s="158"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13452,9 +13512,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="160"/>
-      <c r="D1027" s="161"/>
-      <c r="E1027" s="161"/>
+      <c r="C1027" s="157"/>
+      <c r="D1027" s="158"/>
+      <c r="E1027" s="158"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13605,9 +13665,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="160"/>
-      <c r="D1044" s="161"/>
-      <c r="E1044" s="161"/>
+      <c r="C1044" s="157"/>
+      <c r="D1044" s="158"/>
+      <c r="E1044" s="158"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -13758,9 +13818,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="160"/>
-      <c r="D1061" s="161"/>
-      <c r="E1061" s="161"/>
+      <c r="C1061" s="157"/>
+      <c r="D1061" s="158"/>
+      <c r="E1061" s="158"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -13911,9 +13971,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="160"/>
-      <c r="D1078" s="161"/>
-      <c r="E1078" s="161"/>
+      <c r="C1078" s="157"/>
+      <c r="D1078" s="158"/>
+      <c r="E1078" s="158"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14064,18 +14124,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="170"/>
-      <c r="D1095" s="171"/>
-      <c r="E1095" s="171"/>
+      <c r="C1095" s="167"/>
+      <c r="D1095" s="168"/>
+      <c r="E1095" s="168"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="160"/>
-      <c r="D1096" s="161"/>
-      <c r="E1096" s="161"/>
+      <c r="C1096" s="157"/>
+      <c r="D1096" s="158"/>
+      <c r="E1096" s="158"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14226,9 +14286,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="162"/>
-      <c r="D1113" s="163"/>
-      <c r="E1113" s="163"/>
+      <c r="C1113" s="159"/>
+      <c r="D1113" s="160"/>
+      <c r="E1113" s="160"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14379,9 +14439,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="160"/>
-      <c r="D1130" s="161"/>
-      <c r="E1130" s="161"/>
+      <c r="C1130" s="157"/>
+      <c r="D1130" s="158"/>
+      <c r="E1130" s="158"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14532,9 +14592,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="160"/>
-      <c r="D1147" s="161"/>
-      <c r="E1147" s="161"/>
+      <c r="C1147" s="157"/>
+      <c r="D1147" s="158"/>
+      <c r="E1147" s="158"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -14685,9 +14745,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="160"/>
-      <c r="D1164" s="161"/>
-      <c r="E1164" s="161"/>
+      <c r="C1164" s="157"/>
+      <c r="D1164" s="158"/>
+      <c r="E1164" s="158"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -14838,9 +14898,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="160"/>
-      <c r="D1181" s="161"/>
-      <c r="E1181" s="161"/>
+      <c r="C1181" s="157"/>
+      <c r="D1181" s="158"/>
+      <c r="E1181" s="158"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -14991,9 +15051,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="160"/>
-      <c r="D1198" s="161"/>
-      <c r="E1198" s="161"/>
+      <c r="C1198" s="157"/>
+      <c r="D1198" s="158"/>
+      <c r="E1198" s="158"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15144,9 +15204,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="160"/>
-      <c r="D1215" s="161"/>
-      <c r="E1215" s="161"/>
+      <c r="C1215" s="157"/>
+      <c r="D1215" s="158"/>
+      <c r="E1215" s="158"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15297,9 +15357,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="160"/>
-      <c r="D1232" s="161"/>
-      <c r="E1232" s="161"/>
+      <c r="C1232" s="157"/>
+      <c r="D1232" s="158"/>
+      <c r="E1232" s="158"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15450,9 +15510,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="160"/>
-      <c r="D1249" s="161"/>
-      <c r="E1249" s="161"/>
+      <c r="C1249" s="157"/>
+      <c r="D1249" s="158"/>
+      <c r="E1249" s="158"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15603,9 +15663,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="160"/>
-      <c r="D1266" s="161"/>
-      <c r="E1266" s="161"/>
+      <c r="C1266" s="157"/>
+      <c r="D1266" s="158"/>
+      <c r="E1266" s="158"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -15756,9 +15816,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="160"/>
-      <c r="D1283" s="161"/>
-      <c r="E1283" s="161"/>
+      <c r="C1283" s="157"/>
+      <c r="D1283" s="158"/>
+      <c r="E1283" s="158"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -15909,9 +15969,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="160"/>
-      <c r="D1300" s="161"/>
-      <c r="E1300" s="161"/>
+      <c r="C1300" s="157"/>
+      <c r="D1300" s="158"/>
+      <c r="E1300" s="158"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16062,9 +16122,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="160"/>
-      <c r="D1317" s="161"/>
-      <c r="E1317" s="161"/>
+      <c r="C1317" s="157"/>
+      <c r="D1317" s="158"/>
+      <c r="E1317" s="158"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16215,9 +16275,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="160"/>
-      <c r="D1334" s="161"/>
-      <c r="E1334" s="161"/>
+      <c r="C1334" s="157"/>
+      <c r="D1334" s="158"/>
+      <c r="E1334" s="158"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16368,9 +16428,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="160"/>
-      <c r="D1351" s="161"/>
-      <c r="E1351" s="161"/>
+      <c r="C1351" s="157"/>
+      <c r="D1351" s="158"/>
+      <c r="E1351" s="158"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16521,18 +16581,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="172"/>
-      <c r="D1368" s="173"/>
-      <c r="E1368" s="173"/>
+      <c r="C1368" s="165"/>
+      <c r="D1368" s="166"/>
+      <c r="E1368" s="166"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="160"/>
-      <c r="D1369" s="161"/>
-      <c r="E1369" s="161"/>
+      <c r="C1369" s="157"/>
+      <c r="D1369" s="158"/>
+      <c r="E1369" s="158"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -16683,9 +16743,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="162"/>
-      <c r="D1386" s="163"/>
-      <c r="E1386" s="163"/>
+      <c r="C1386" s="159"/>
+      <c r="D1386" s="160"/>
+      <c r="E1386" s="160"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -16836,9 +16896,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="160"/>
-      <c r="D1403" s="161"/>
-      <c r="E1403" s="161"/>
+      <c r="C1403" s="157"/>
+      <c r="D1403" s="158"/>
+      <c r="E1403" s="158"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -16989,9 +17049,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="160"/>
-      <c r="D1420" s="161"/>
-      <c r="E1420" s="161"/>
+      <c r="C1420" s="157"/>
+      <c r="D1420" s="158"/>
+      <c r="E1420" s="158"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17142,9 +17202,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="160"/>
-      <c r="D1437" s="161"/>
-      <c r="E1437" s="161"/>
+      <c r="C1437" s="157"/>
+      <c r="D1437" s="158"/>
+      <c r="E1437" s="158"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17295,9 +17355,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="160"/>
-      <c r="D1454" s="161"/>
-      <c r="E1454" s="161"/>
+      <c r="C1454" s="157"/>
+      <c r="D1454" s="158"/>
+      <c r="E1454" s="158"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17448,9 +17508,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="160"/>
-      <c r="D1471" s="161"/>
-      <c r="E1471" s="161"/>
+      <c r="C1471" s="157"/>
+      <c r="D1471" s="158"/>
+      <c r="E1471" s="158"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17601,9 +17661,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="160"/>
-      <c r="D1488" s="161"/>
-      <c r="E1488" s="161"/>
+      <c r="C1488" s="157"/>
+      <c r="D1488" s="158"/>
+      <c r="E1488" s="158"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -17754,9 +17814,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="160"/>
-      <c r="D1505" s="161"/>
-      <c r="E1505" s="161"/>
+      <c r="C1505" s="157"/>
+      <c r="D1505" s="158"/>
+      <c r="E1505" s="158"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -17907,9 +17967,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="160"/>
-      <c r="D1522" s="161"/>
-      <c r="E1522" s="161"/>
+      <c r="C1522" s="157"/>
+      <c r="D1522" s="158"/>
+      <c r="E1522" s="158"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18060,9 +18120,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="160"/>
-      <c r="D1539" s="161"/>
-      <c r="E1539" s="161"/>
+      <c r="C1539" s="157"/>
+      <c r="D1539" s="158"/>
+      <c r="E1539" s="158"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18213,9 +18273,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="160"/>
-      <c r="D1556" s="161"/>
-      <c r="E1556" s="161"/>
+      <c r="C1556" s="157"/>
+      <c r="D1556" s="158"/>
+      <c r="E1556" s="158"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18366,9 +18426,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="160"/>
-      <c r="D1573" s="161"/>
-      <c r="E1573" s="161"/>
+      <c r="C1573" s="157"/>
+      <c r="D1573" s="158"/>
+      <c r="E1573" s="158"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18519,9 +18579,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="160"/>
-      <c r="D1590" s="161"/>
-      <c r="E1590" s="161"/>
+      <c r="C1590" s="157"/>
+      <c r="D1590" s="158"/>
+      <c r="E1590" s="158"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -18672,9 +18732,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="160"/>
-      <c r="D1607" s="161"/>
-      <c r="E1607" s="161"/>
+      <c r="C1607" s="157"/>
+      <c r="D1607" s="158"/>
+      <c r="E1607" s="158"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -18825,9 +18885,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="160"/>
-      <c r="D1624" s="161"/>
-      <c r="E1624" s="161"/>
+      <c r="C1624" s="157"/>
+      <c r="D1624" s="158"/>
+      <c r="E1624" s="158"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -18978,18 +19038,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="174"/>
-      <c r="D1641" s="175"/>
-      <c r="E1641" s="175"/>
+      <c r="C1641" s="163"/>
+      <c r="D1641" s="164"/>
+      <c r="E1641" s="164"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="160"/>
-      <c r="D1642" s="161"/>
-      <c r="E1642" s="161"/>
+      <c r="C1642" s="157"/>
+      <c r="D1642" s="158"/>
+      <c r="E1642" s="158"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19140,9 +19200,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="162"/>
-      <c r="D1659" s="163"/>
-      <c r="E1659" s="163"/>
+      <c r="C1659" s="159"/>
+      <c r="D1659" s="160"/>
+      <c r="E1659" s="160"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19293,9 +19353,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="160"/>
-      <c r="D1676" s="161"/>
-      <c r="E1676" s="161"/>
+      <c r="C1676" s="157"/>
+      <c r="D1676" s="158"/>
+      <c r="E1676" s="158"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19446,9 +19506,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="160"/>
-      <c r="D1693" s="161"/>
-      <c r="E1693" s="161"/>
+      <c r="C1693" s="157"/>
+      <c r="D1693" s="158"/>
+      <c r="E1693" s="158"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19599,9 +19659,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="160"/>
-      <c r="D1710" s="161"/>
-      <c r="E1710" s="161"/>
+      <c r="C1710" s="157"/>
+      <c r="D1710" s="158"/>
+      <c r="E1710" s="158"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -19752,9 +19812,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="160"/>
-      <c r="D1727" s="161"/>
-      <c r="E1727" s="161"/>
+      <c r="C1727" s="157"/>
+      <c r="D1727" s="158"/>
+      <c r="E1727" s="158"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -19905,9 +19965,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="160"/>
-      <c r="D1744" s="161"/>
-      <c r="E1744" s="161"/>
+      <c r="C1744" s="157"/>
+      <c r="D1744" s="158"/>
+      <c r="E1744" s="158"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20058,9 +20118,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="160"/>
-      <c r="D1761" s="161"/>
-      <c r="E1761" s="161"/>
+      <c r="C1761" s="157"/>
+      <c r="D1761" s="158"/>
+      <c r="E1761" s="158"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20211,9 +20271,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="160"/>
-      <c r="D1778" s="161"/>
-      <c r="E1778" s="161"/>
+      <c r="C1778" s="157"/>
+      <c r="D1778" s="158"/>
+      <c r="E1778" s="158"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20364,9 +20424,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="160"/>
-      <c r="D1795" s="161"/>
-      <c r="E1795" s="161"/>
+      <c r="C1795" s="157"/>
+      <c r="D1795" s="158"/>
+      <c r="E1795" s="158"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20517,9 +20577,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="160"/>
-      <c r="D1812" s="161"/>
-      <c r="E1812" s="161"/>
+      <c r="C1812" s="157"/>
+      <c r="D1812" s="158"/>
+      <c r="E1812" s="158"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -20670,9 +20730,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="160"/>
-      <c r="D1829" s="161"/>
-      <c r="E1829" s="161"/>
+      <c r="C1829" s="157"/>
+      <c r="D1829" s="158"/>
+      <c r="E1829" s="158"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -20823,9 +20883,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="160"/>
-      <c r="D1846" s="161"/>
-      <c r="E1846" s="161"/>
+      <c r="C1846" s="157"/>
+      <c r="D1846" s="158"/>
+      <c r="E1846" s="158"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -20976,9 +21036,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="160"/>
-      <c r="D1863" s="161"/>
-      <c r="E1863" s="161"/>
+      <c r="C1863" s="157"/>
+      <c r="D1863" s="158"/>
+      <c r="E1863" s="158"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21129,9 +21189,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="160"/>
-      <c r="D1880" s="161"/>
-      <c r="E1880" s="161"/>
+      <c r="C1880" s="157"/>
+      <c r="D1880" s="158"/>
+      <c r="E1880" s="158"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21282,9 +21342,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="160"/>
-      <c r="D1897" s="161"/>
-      <c r="E1897" s="161"/>
+      <c r="C1897" s="157"/>
+      <c r="D1897" s="158"/>
+      <c r="E1897" s="158"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21435,18 +21495,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="176"/>
-      <c r="D1914" s="177"/>
-      <c r="E1914" s="177"/>
+      <c r="C1914" s="161"/>
+      <c r="D1914" s="162"/>
+      <c r="E1914" s="162"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="160"/>
-      <c r="D1915" s="161"/>
-      <c r="E1915" s="161"/>
+      <c r="C1915" s="157"/>
+      <c r="D1915" s="158"/>
+      <c r="E1915" s="158"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21597,9 +21657,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="162"/>
-      <c r="D1932" s="163"/>
-      <c r="E1932" s="163"/>
+      <c r="C1932" s="159"/>
+      <c r="D1932" s="160"/>
+      <c r="E1932" s="160"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -21750,9 +21810,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="160"/>
-      <c r="D1949" s="161"/>
-      <c r="E1949" s="161"/>
+      <c r="C1949" s="157"/>
+      <c r="D1949" s="158"/>
+      <c r="E1949" s="158"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -21903,9 +21963,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="160"/>
-      <c r="D1966" s="161"/>
-      <c r="E1966" s="161"/>
+      <c r="C1966" s="157"/>
+      <c r="D1966" s="158"/>
+      <c r="E1966" s="158"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22056,9 +22116,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="160"/>
-      <c r="D1983" s="161"/>
-      <c r="E1983" s="161"/>
+      <c r="C1983" s="157"/>
+      <c r="D1983" s="158"/>
+      <c r="E1983" s="158"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22209,9 +22269,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="160"/>
-      <c r="D2000" s="161"/>
-      <c r="E2000" s="161"/>
+      <c r="C2000" s="157"/>
+      <c r="D2000" s="158"/>
+      <c r="E2000" s="158"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22362,9 +22422,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="160"/>
-      <c r="D2017" s="161"/>
-      <c r="E2017" s="161"/>
+      <c r="C2017" s="157"/>
+      <c r="D2017" s="158"/>
+      <c r="E2017" s="158"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22515,9 +22575,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="160"/>
-      <c r="D2034" s="161"/>
-      <c r="E2034" s="161"/>
+      <c r="C2034" s="157"/>
+      <c r="D2034" s="158"/>
+      <c r="E2034" s="158"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -22668,9 +22728,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="160"/>
-      <c r="D2051" s="161"/>
-      <c r="E2051" s="161"/>
+      <c r="C2051" s="157"/>
+      <c r="D2051" s="158"/>
+      <c r="E2051" s="158"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -22821,9 +22881,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="160"/>
-      <c r="D2068" s="161"/>
-      <c r="E2068" s="161"/>
+      <c r="C2068" s="157"/>
+      <c r="D2068" s="158"/>
+      <c r="E2068" s="158"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -22974,9 +23034,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="160"/>
-      <c r="D2085" s="161"/>
-      <c r="E2085" s="161"/>
+      <c r="C2085" s="157"/>
+      <c r="D2085" s="158"/>
+      <c r="E2085" s="158"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23127,9 +23187,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="160"/>
-      <c r="D2102" s="161"/>
-      <c r="E2102" s="161"/>
+      <c r="C2102" s="157"/>
+      <c r="D2102" s="158"/>
+      <c r="E2102" s="158"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23280,9 +23340,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="160"/>
-      <c r="D2119" s="161"/>
-      <c r="E2119" s="161"/>
+      <c r="C2119" s="157"/>
+      <c r="D2119" s="158"/>
+      <c r="E2119" s="158"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23433,9 +23493,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="160"/>
-      <c r="D2136" s="161"/>
-      <c r="E2136" s="161"/>
+      <c r="C2136" s="157"/>
+      <c r="D2136" s="158"/>
+      <c r="E2136" s="158"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23586,9 +23646,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="160"/>
-      <c r="D2153" s="161"/>
-      <c r="E2153" s="161"/>
+      <c r="C2153" s="157"/>
+      <c r="D2153" s="158"/>
+      <c r="E2153" s="158"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -23739,9 +23799,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="160"/>
-      <c r="D2170" s="161"/>
-      <c r="E2170" s="161"/>
+      <c r="C2170" s="157"/>
+      <c r="D2170" s="158"/>
+      <c r="E2170" s="158"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -23889,15 +23949,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -23910,124 +24077,17 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24778,7 +24838,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -24989,7 +25049,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25209,9 +25269,9 @@
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
-      <c r="C20" s="132">
+      <c r="C20" s="132" t="str">
         <f>FrameCounts!B21</f>
-        <v>0</v>
+        <v>Bimmy Appears</v>
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -25262,7 +25322,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25284,150 +25344,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="202" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="204"/>
+      <c r="B1" s="203"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="209" t="s">
+      <c r="A2" s="199" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="210"/>
+      <c r="B2" s="200"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="211" t="s">
+      <c r="A3" s="201" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="210"/>
+      <c r="B3" s="200"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="207"/>
-      <c r="B4" s="208"/>
+      <c r="A4" s="206"/>
+      <c r="B4" s="207"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="205" t="s">
+      <c r="A5" s="204" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="206"/>
+      <c r="B5" s="205"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="197" t="s">
+      <c r="A7" s="210" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="198"/>
+      <c r="B7" s="211"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="199" t="s">
+      <c r="A9" s="208" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="200"/>
+      <c r="B9" s="209"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="201"/>
-      <c r="B10" s="202"/>
+      <c r="A10" s="195"/>
+      <c r="B10" s="196"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="193" t="s">
+      <c r="A11" s="197" t="s">
         <v>196</v>
       </c>
-      <c r="B11" s="194"/>
+      <c r="B11" s="198"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="193" t="s">
+      <c r="A12" s="197" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="194"/>
+      <c r="B12" s="198"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="193" t="s">
+      <c r="A13" s="197" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="194"/>
+      <c r="B13" s="198"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="193" t="s">
+      <c r="A14" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="194"/>
+      <c r="B14" s="198"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="193" t="s">
+      <c r="A15" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="194"/>
+      <c r="B15" s="198"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="193" t="s">
+      <c r="A16" s="197" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="194"/>
+      <c r="B16" s="198"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="195" t="s">
+      <c r="A17" s="193" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="196"/>
+      <c r="B17" s="194"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="197" t="s">
+      <c r="A19" s="210" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="198"/>
+      <c r="B19" s="211"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="199" t="s">
+      <c r="A21" s="208" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="200"/>
+      <c r="B21" s="209"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="201"/>
-      <c r="B22" s="202"/>
+      <c r="A22" s="195"/>
+      <c r="B22" s="196"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="193" t="s">
+      <c r="A23" s="197" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="194"/>
+      <c r="B23" s="198"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="193"/>
-      <c r="B24" s="194"/>
+      <c r="A24" s="197"/>
+      <c r="B24" s="198"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="193" t="s">
+      <c r="A25" s="197" t="s">
         <v>208</v>
       </c>
-      <c r="B25" s="194"/>
+      <c r="B25" s="198"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="193" t="s">
+      <c r="A26" s="197" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="194"/>
+      <c r="B26" s="198"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="195"/>
-      <c r="B27" s="196"/>
+      <c r="A27" s="193"/>
+      <c r="B27" s="194"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25438,19 +25511,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>